<commit_message>
updated energy structures for better integration and standardization of energy demands and implementation of efficiencies.
</commit_message>
<xml_diff>
--- a/ref/ipcc_data_tables_and_derivations/AFOLU/afolu_c2_general_use_tables.xlsx
+++ b/ref/ipcc_data_tables_and_derivations/AFOLU/afolu_c2_general_use_tables.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ipcc_data_tables_and_derivations/AFOLU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0A74E9-BA31-F645-8C3B-4813831E6729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC9B166-DA97-2849-A8EC-3749F1BE71F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6140" yWindow="460" windowWidth="24220" windowHeight="17520" xr2:uid="{0F7B3AC4-6872-894F-9C5F-CA57A58590FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 2.3" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -490,7 +490,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>